<commit_message>
updated activity Tracker week 4
</commit_message>
<xml_diff>
--- a/documents/Activity Tracker.xlsx
+++ b/documents/Activity Tracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17301"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="87">
   <si>
     <t>Week-wise-Effort</t>
   </si>
@@ -357,6 +357,42 @@
   </si>
   <si>
     <t>Tutorials/Self Learning</t>
+  </si>
+  <si>
+    <t>Menu Initialization</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>Item Class Creation</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Firebase database research</t>
+  </si>
+  <si>
+    <t>Edgar</t>
+  </si>
+  <si>
+    <t>Android Object Creation</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Yelp Range Request</t>
+  </si>
+  <si>
+    <t>Colton</t>
+  </si>
+  <si>
+    <t>Swipe Functionality</t>
+  </si>
+  <si>
+    <t>Brashad</t>
   </si>
 </sst>
 </file>
@@ -780,6 +816,27 @@
                 <c:pt idx="11">
                   <c:v>Week 4</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>Meetings</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Menu Initialization</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Item Class Creation</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Firebase database research</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Android Object Creation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Yelp Range Request</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Swipe Functionality</c:v>
+                </c:pt>
                 <c:pt idx="22">
                   <c:v>Week 5</c:v>
                 </c:pt>
@@ -2011,7 +2068,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>18</c:v>
@@ -2614,7 +2671,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>18</c:v>
@@ -2912,7 +2969,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2933,7 +2990,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3159,7 +3216,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2068" name="Chart 2"/>
+        <xdr:cNvPr id="2068" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3191,7 +3254,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2069" name="Chart 3"/>
+        <xdr:cNvPr id="2069" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000015080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3223,7 +3292,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2070" name="Chart 4"/>
+        <xdr:cNvPr id="2070" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000016080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3255,7 +3330,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2071" name="Chart 5"/>
+        <xdr:cNvPr id="2071" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000017080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3287,7 +3368,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2072" name="Chart 6"/>
+        <xdr:cNvPr id="2072" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000018080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3319,7 +3406,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2073" name="Chart 7"/>
+        <xdr:cNvPr id="2073" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000019080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3723,24 +3816,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J269"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="11" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="48.28515625" customWidth="1"/>
-    <col min="9" max="10" width="11.28515625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="48.33203125" customWidth="1"/>
+    <col min="9" max="10" width="11.33203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="12" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>39</v>
       </c>
@@ -3772,7 +3865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="33" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="33" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>67</v>
       </c>
@@ -3784,7 +3877,7 @@
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
-    <row r="3" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -3806,7 +3899,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>71</v>
       </c>
@@ -3838,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
@@ -3870,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
@@ -3902,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -3922,7 +4015,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -3942,7 +4035,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
@@ -3962,7 +4055,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -3982,7 +4075,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -4002,7 +4095,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -4022,7 +4115,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="G13" s="30" t="s">
@@ -4037,7 +4130,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="G14" s="30" t="s">
@@ -4052,7 +4145,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="3" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -4064,32 +4157,54 @@
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
     </row>
-    <row r="16" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+    <row r="16" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="8">
+        <v>4</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="8">
+        <v>6</v>
+      </c>
+      <c r="F16" s="8">
+        <v>6</v>
+      </c>
       <c r="G16" s="29" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="7"/>
-      <c r="I16" s="18" t="str">
+      <c r="I16" s="18">
         <f t="shared" ref="I16:I25" si="2">IF(OR(E16="", F16=""), "", E16-F16)</f>
-        <v/>
-      </c>
-      <c r="J16" s="18" t="str">
+        <v>0</v>
+      </c>
+      <c r="J16" s="18">
         <f t="shared" ref="J16:J25" si="3">IF(OR(I16="",F16=0),"",ABS(I16)/F16*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="8">
+        <v>4</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="8">
+        <v>5</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="29" t="s">
         <v>69</v>
@@ -4104,12 +4219,22 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+    <row r="18" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="8">
+        <v>4</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="8">
+        <v>5</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="29" t="s">
         <v>69</v>
@@ -4124,12 +4249,22 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+    <row r="19" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="8">
+        <v>4</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="8">
+        <v>5</v>
+      </c>
       <c r="F19" s="8"/>
       <c r="G19" s="29" t="s">
         <v>69</v>
@@ -4144,12 +4279,22 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+    <row r="20" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="8">
+        <v>4</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="8">
+        <v>5</v>
+      </c>
       <c r="F20" s="8"/>
       <c r="G20" s="29" t="s">
         <v>69</v>
@@ -4164,12 +4309,22 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+    <row r="21" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="8">
+        <v>4</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="8">
+        <v>5</v>
+      </c>
       <c r="F21" s="8"/>
       <c r="G21" s="29" t="s">
         <v>69</v>
@@ -4184,12 +4339,22 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+    <row r="22" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="8">
+        <v>4</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="8">
+        <v>5</v>
+      </c>
       <c r="F22" s="8"/>
       <c r="G22" s="29" t="s">
         <v>69</v>
@@ -4204,7 +4369,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -4224,7 +4389,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -4240,7 +4405,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -4260,7 +4425,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="3" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -4272,7 +4437,7 @@
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="G27" s="30" t="s">
@@ -4287,7 +4452,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="G28" s="30" t="s">
@@ -4302,7 +4467,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="G29" s="30" t="s">
@@ -4317,7 +4482,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="G30" s="30" t="s">
@@ -4332,7 +4497,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="G31" s="30" t="s">
@@ -4347,7 +4512,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="G32" s="30" t="s">
@@ -4362,7 +4527,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G33" s="30" t="s">
         <v>69</v>
       </c>
@@ -4375,7 +4540,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -4395,7 +4560,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G35" s="30" t="s">
         <v>69</v>
       </c>
@@ -4408,7 +4573,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G36" s="30" t="s">
         <v>69</v>
       </c>
@@ -4421,7 +4586,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G37" s="30" t="s">
         <v>69</v>
       </c>
@@ -4434,7 +4599,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G38" s="30" t="s">
         <v>69</v>
       </c>
@@ -4447,7 +4612,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G39" s="30" t="s">
         <v>69</v>
       </c>
@@ -4460,7 +4625,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G40" s="30" t="s">
         <v>69</v>
       </c>
@@ -4473,7 +4638,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G41" s="30" t="s">
         <v>69</v>
       </c>
@@ -4486,7 +4651,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G42" s="30" t="s">
         <v>69</v>
       </c>
@@ -4499,7 +4664,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>31</v>
       </c>
@@ -4519,7 +4684,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G44" s="30" t="s">
         <v>69</v>
       </c>
@@ -4532,7 +4697,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G45" s="30" t="s">
         <v>69</v>
       </c>
@@ -4545,7 +4710,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G46" s="30" t="s">
         <v>69</v>
       </c>
@@ -4558,7 +4723,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G47" s="30" t="s">
         <v>69</v>
       </c>
@@ -4571,7 +4736,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G48" s="30" t="s">
         <v>69</v>
       </c>
@@ -4584,7 +4749,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G49" s="30" t="s">
         <v>69</v>
       </c>
@@ -4597,28 +4762,28 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G50" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G51" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I51" s="18"/>
       <c r="J51" s="18"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G52" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I52" s="18"/>
       <c r="J52" s="18"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G53" s="30" t="s">
         <v>69</v>
       </c>
@@ -4631,11 +4796,11 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>32</v>
       </c>
@@ -4655,7 +4820,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G56" s="30" t="s">
         <v>69</v>
       </c>
@@ -4668,7 +4833,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G57" s="30" t="s">
         <v>69</v>
       </c>
@@ -4681,7 +4846,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G58" s="30" t="s">
         <v>69</v>
       </c>
@@ -4694,7 +4859,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G59" s="30" t="s">
         <v>69</v>
       </c>
@@ -4707,7 +4872,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G60" s="30" t="s">
         <v>69</v>
       </c>
@@ -4720,7 +4885,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G61" s="30" t="s">
         <v>69</v>
       </c>
@@ -4733,7 +4898,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G62" s="30" t="s">
         <v>69</v>
       </c>
@@ -4746,7 +4911,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G63" s="30" t="s">
         <v>69</v>
       </c>
@@ -4759,7 +4924,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -4779,7 +4944,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G65" s="30" t="s">
         <v>69</v>
       </c>
@@ -4792,7 +4957,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G66" s="30" t="s">
         <v>69</v>
       </c>
@@ -4805,7 +4970,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G67" s="30" t="s">
         <v>69</v>
       </c>
@@ -4818,7 +4983,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G68" s="30" t="s">
         <v>69</v>
       </c>
@@ -4831,7 +4996,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G69" s="30" t="s">
         <v>69</v>
       </c>
@@ -4844,7 +5009,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G70" s="30" t="s">
         <v>69</v>
       </c>
@@ -4857,7 +5022,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G71" s="30" t="s">
         <v>69</v>
       </c>
@@ -4870,7 +5035,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G72" s="30" t="s">
         <v>69</v>
       </c>
@@ -4883,7 +5048,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G73" s="30" t="s">
         <v>69</v>
       </c>
@@ -4896,7 +5061,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G74" s="30" t="s">
         <v>69</v>
       </c>
@@ -4909,7 +5074,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G75" s="30" t="s">
         <v>69</v>
       </c>
@@ -4922,7 +5087,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G76" s="30" t="s">
         <v>69</v>
       </c>
@@ -4935,7 +5100,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G77" s="30" t="s">
         <v>69</v>
       </c>
@@ -4948,7 +5113,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G78" s="30" t="s">
         <v>69</v>
       </c>
@@ -4961,7 +5126,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I79" s="18" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4971,7 +5136,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
@@ -4991,7 +5156,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G81" s="30" t="s">
         <v>69</v>
       </c>
@@ -5004,7 +5169,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G82" s="30" t="s">
         <v>69</v>
       </c>
@@ -5017,35 +5182,35 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G83" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I83" s="18"/>
       <c r="J83" s="18"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G84" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I84" s="18"/>
       <c r="J84" s="18"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G85" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I85" s="18"/>
       <c r="J85" s="18"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G86" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I86" s="18"/>
       <c r="J86" s="18"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G87" s="30" t="s">
         <v>69</v>
       </c>
@@ -5058,35 +5223,35 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G88" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I88" s="18"/>
       <c r="J88" s="18"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G89" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I89" s="18"/>
       <c r="J89" s="18"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G90" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I90" s="18"/>
       <c r="J90" s="18"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G91" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I91" s="18"/>
       <c r="J91" s="18"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G92" s="30" t="s">
         <v>69</v>
       </c>
@@ -5099,14 +5264,14 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G93" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I93" s="18"/>
       <c r="J93" s="18"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G94" s="30" t="s">
         <v>69</v>
       </c>
@@ -5119,7 +5284,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G95" s="30" t="s">
         <v>69</v>
       </c>
@@ -5132,7 +5297,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>35</v>
       </c>
@@ -5152,7 +5317,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G97" s="30" t="s">
         <v>69</v>
       </c>
@@ -5165,7 +5330,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G98" s="30" t="s">
         <v>69</v>
       </c>
@@ -5178,7 +5343,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G99" s="30" t="s">
         <v>69</v>
       </c>
@@ -5191,49 +5356,49 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G100" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I100" s="18"/>
       <c r="J100" s="18"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G101" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I101" s="18"/>
       <c r="J101" s="18"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G102" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I102" s="18"/>
       <c r="J102" s="18"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G103" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I103" s="18"/>
       <c r="J103" s="18"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G104" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I104" s="18"/>
       <c r="J104" s="18"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G105" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I105" s="18"/>
       <c r="J105" s="18"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G106" s="30" t="s">
         <v>69</v>
       </c>
@@ -5246,7 +5411,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G107" s="30" t="s">
         <v>69</v>
       </c>
@@ -5259,7 +5424,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G108" s="30" t="s">
         <v>69</v>
       </c>
@@ -5272,7 +5437,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>36</v>
       </c>
@@ -5292,7 +5457,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G110" s="30" t="s">
         <v>70</v>
       </c>
@@ -5305,14 +5470,14 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G111" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I111" s="18"/>
       <c r="J111" s="18"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G112" s="30" t="s">
         <v>69</v>
       </c>
@@ -5325,7 +5490,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G113" s="30" t="s">
         <v>69</v>
       </c>
@@ -5338,7 +5503,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G114" s="30" t="s">
         <v>69</v>
       </c>
@@ -5351,7 +5516,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I115" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5361,7 +5526,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>37</v>
       </c>
@@ -5374,7 +5539,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I117" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5384,7 +5549,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I118" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5394,7 +5559,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I119" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5404,7 +5569,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I120" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5414,7 +5579,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I121" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5424,7 +5589,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I122" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5434,7 +5599,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I123" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5444,7 +5609,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I124" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5454,7 +5619,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I125" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5464,7 +5629,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I126" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5474,7 +5639,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I127" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5484,7 +5649,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I128" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5494,7 +5659,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I129" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5504,7 +5669,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I130" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5514,7 +5679,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I131" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5524,7 +5689,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I132" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5534,7 +5699,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I133" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5544,7 +5709,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I134" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5554,7 +5719,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I135" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5564,7 +5729,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I136" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5574,7 +5739,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I137" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5584,7 +5749,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I138" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5594,7 +5759,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I139" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5604,7 +5769,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I140" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5614,7 +5779,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I141" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5624,7 +5789,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I142" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5634,7 +5799,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I143" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5644,7 +5809,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I144" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5654,7 +5819,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I145" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5664,7 +5829,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I146" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5674,7 +5839,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I147" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5684,7 +5849,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I148" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5694,7 +5859,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I149" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5704,7 +5869,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I150" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5714,7 +5879,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I151" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5724,7 +5889,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I152" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5734,7 +5899,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I153" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5744,7 +5909,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I154" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5754,7 +5919,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I155" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5764,7 +5929,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I156" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -5774,7 +5939,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I157" s="18" t="str">
         <f t="shared" ref="I157:I220" si="8">IF(OR(E157="", F157=""), "", E157-F157)</f>
         <v/>
@@ -5784,7 +5949,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I158" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5794,7 +5959,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I159" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5804,7 +5969,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I160" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5814,7 +5979,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I161" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5824,7 +5989,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I162" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5834,7 +5999,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I163" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5844,7 +6009,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I164" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5854,7 +6019,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I165" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5864,7 +6029,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I166" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5874,7 +6039,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I167" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5884,7 +6049,7 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I168" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5894,7 +6059,7 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I169" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5904,7 +6069,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I170" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5914,7 +6079,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I171" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5924,7 +6089,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I172" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5934,7 +6099,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I173" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5944,7 +6109,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I174" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5954,7 +6119,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I175" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5964,7 +6129,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I176" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5974,7 +6139,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I177" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5984,7 +6149,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I178" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5994,7 +6159,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I179" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6004,7 +6169,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="180" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I180" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6014,7 +6179,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="181" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I181" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6024,7 +6189,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I182" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6034,7 +6199,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I183" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6044,7 +6209,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I184" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6054,7 +6219,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="185" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I185" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6064,7 +6229,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="186" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I186" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6074,7 +6239,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I187" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6084,7 +6249,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I188" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6094,7 +6259,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I189" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6104,7 +6269,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="190" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I190" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6114,7 +6279,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I191" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6124,7 +6289,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I192" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6134,7 +6299,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I193" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6144,7 +6309,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I194" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6154,7 +6319,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I195" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6164,7 +6329,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I196" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6174,7 +6339,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I197" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6184,7 +6349,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I198" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6194,7 +6359,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I199" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6204,7 +6369,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I200" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6214,7 +6379,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I201" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6224,7 +6389,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I202" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6234,7 +6399,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I203" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6244,7 +6409,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I204" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6254,7 +6419,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I205" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6264,7 +6429,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I206" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6274,7 +6439,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I207" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6284,7 +6449,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I208" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6294,7 +6459,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="209" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I209" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6304,7 +6469,7 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="210" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I210" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6314,7 +6479,7 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="211" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I211" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6324,7 +6489,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="212" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I212" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6334,7 +6499,7 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="213" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I213" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6344,7 +6509,7 @@
         <v/>
       </c>
     </row>
-    <row r="214" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="214" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I214" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6354,7 +6519,7 @@
         <v/>
       </c>
     </row>
-    <row r="215" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="215" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I215" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6364,7 +6529,7 @@
         <v/>
       </c>
     </row>
-    <row r="216" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="216" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I216" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6374,7 +6539,7 @@
         <v/>
       </c>
     </row>
-    <row r="217" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="217" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I217" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6384,7 +6549,7 @@
         <v/>
       </c>
     </row>
-    <row r="218" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="218" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I218" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6394,7 +6559,7 @@
         <v/>
       </c>
     </row>
-    <row r="219" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="219" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I219" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6404,7 +6569,7 @@
         <v/>
       </c>
     </row>
-    <row r="220" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="220" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I220" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -6414,7 +6579,7 @@
         <v/>
       </c>
     </row>
-    <row r="221" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="221" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I221" s="18" t="str">
         <f t="shared" ref="I221:I262" si="10">IF(OR(E221="", F221=""), "", E221-F221)</f>
         <v/>
@@ -6424,7 +6589,7 @@
         <v/>
       </c>
     </row>
-    <row r="222" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="222" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I222" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6434,7 +6599,7 @@
         <v/>
       </c>
     </row>
-    <row r="223" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="223" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I223" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6444,7 +6609,7 @@
         <v/>
       </c>
     </row>
-    <row r="224" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="224" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I224" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6454,7 +6619,7 @@
         <v/>
       </c>
     </row>
-    <row r="225" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="225" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I225" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6464,7 +6629,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="226" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I226" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6474,7 +6639,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="227" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I227" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6484,7 +6649,7 @@
         <v/>
       </c>
     </row>
-    <row r="228" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="228" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I228" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6494,7 +6659,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="229" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I229" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6504,7 +6669,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="230" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I230" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6514,7 +6679,7 @@
         <v/>
       </c>
     </row>
-    <row r="231" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="231" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I231" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6524,7 +6689,7 @@
         <v/>
       </c>
     </row>
-    <row r="232" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="232" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I232" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6534,7 +6699,7 @@
         <v/>
       </c>
     </row>
-    <row r="233" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="233" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I233" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6544,7 +6709,7 @@
         <v/>
       </c>
     </row>
-    <row r="234" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="234" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I234" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6554,7 +6719,7 @@
         <v/>
       </c>
     </row>
-    <row r="235" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="235" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I235" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6564,7 +6729,7 @@
         <v/>
       </c>
     </row>
-    <row r="236" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="236" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I236" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6574,7 +6739,7 @@
         <v/>
       </c>
     </row>
-    <row r="237" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="237" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I237" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6584,7 +6749,7 @@
         <v/>
       </c>
     </row>
-    <row r="238" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="238" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I238" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6594,7 +6759,7 @@
         <v/>
       </c>
     </row>
-    <row r="239" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="239" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I239" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6604,7 +6769,7 @@
         <v/>
       </c>
     </row>
-    <row r="240" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="240" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I240" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6614,7 +6779,7 @@
         <v/>
       </c>
     </row>
-    <row r="241" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="241" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I241" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6624,7 +6789,7 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="242" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I242" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6634,7 +6799,7 @@
         <v/>
       </c>
     </row>
-    <row r="243" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="243" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I243" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6644,7 +6809,7 @@
         <v/>
       </c>
     </row>
-    <row r="244" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="244" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I244" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6654,7 +6819,7 @@
         <v/>
       </c>
     </row>
-    <row r="245" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="245" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I245" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6664,7 +6829,7 @@
         <v/>
       </c>
     </row>
-    <row r="246" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="246" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I246" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6674,7 +6839,7 @@
         <v/>
       </c>
     </row>
-    <row r="247" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="247" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I247" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6684,7 +6849,7 @@
         <v/>
       </c>
     </row>
-    <row r="248" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="248" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I248" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6694,7 +6859,7 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="249" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I249" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6704,7 +6869,7 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="250" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I250" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6714,7 +6879,7 @@
         <v/>
       </c>
     </row>
-    <row r="251" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="251" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I251" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6724,7 +6889,7 @@
         <v/>
       </c>
     </row>
-    <row r="252" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="252" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I252" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6734,7 +6899,7 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="253" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I253" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6744,7 +6909,7 @@
         <v/>
       </c>
     </row>
-    <row r="254" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="254" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I254" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6754,7 +6919,7 @@
         <v/>
       </c>
     </row>
-    <row r="255" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="255" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I255" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6764,7 +6929,7 @@
         <v/>
       </c>
     </row>
-    <row r="256" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="256" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I256" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6774,7 +6939,7 @@
         <v/>
       </c>
     </row>
-    <row r="257" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="257" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I257" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6784,7 +6949,7 @@
         <v/>
       </c>
     </row>
-    <row r="258" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="258" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I258" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6794,7 +6959,7 @@
         <v/>
       </c>
     </row>
-    <row r="259" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="259" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I259" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6804,7 +6969,7 @@
         <v/>
       </c>
     </row>
-    <row r="260" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="260" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I260" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6814,7 +6979,7 @@
         <v/>
       </c>
     </row>
-    <row r="261" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="261" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I261" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6824,7 +6989,7 @@
         <v/>
       </c>
     </row>
-    <row r="262" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="262" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I262" s="18" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6834,43 +6999,43 @@
         <v/>
       </c>
     </row>
-    <row r="263" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="263" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J263" s="18" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="264" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="264" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J264" s="18" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="265" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="265" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J265" s="18" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="266" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="266" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J266" s="18" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="267" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="267" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J267" s="18" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="268" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="268" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J268" s="18" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="269" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="269" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J269" s="18" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -6918,21 +7083,21 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="23" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="23" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="23" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="23" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="23" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="23" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" style="23" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="23" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="23" customWidth="1"/>
+    <col min="10" max="11" width="9.109375" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="16" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="16" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="20"/>
       <c r="B1" s="21" t="s">
         <v>12</v>
@@ -6947,7 +7112,7 @@
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
     </row>
-    <row r="2" spans="1:11" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="15" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -6970,7 +7135,7 @@
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
     </row>
-    <row r="3" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -6983,7 +7148,7 @@
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
@@ -6998,7 +7163,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>54</v>
       </c>
@@ -7031,7 +7196,7 @@
       </c>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>1</v>
       </c>
@@ -7064,7 +7229,7 @@
       </c>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -7077,12 +7242,12 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>1</v>
       </c>
@@ -7104,7 +7269,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>2</v>
       </c>
@@ -7126,7 +7291,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>3</v>
       </c>
@@ -7148,7 +7313,7 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>4</v>
       </c>
@@ -7162,7 +7327,7 @@
       </c>
       <c r="F12" s="24">
         <f>DCOUNT(Activities!A:J,"Estimation Error %",D5:D6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="25">
         <f t="shared" si="0"/>
@@ -7170,7 +7335,7 @@
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>5</v>
       </c>
@@ -7192,7 +7357,7 @@
       </c>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>6</v>
       </c>
@@ -7214,7 +7379,7 @@
       </c>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>7</v>
       </c>
@@ -7236,7 +7401,7 @@
       </c>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>8</v>
       </c>
@@ -7258,7 +7423,7 @@
       </c>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>9</v>
       </c>
@@ -7280,7 +7445,7 @@
       </c>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>10</v>
       </c>
@@ -7302,7 +7467,7 @@
       </c>
       <c r="H18" s="24"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>38</v>
       </c>
@@ -7310,7 +7475,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>46</v>
       </c>
@@ -7319,7 +7484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>50</v>
       </c>
@@ -7328,7 +7493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>49</v>
       </c>
@@ -7337,7 +7502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>48</v>
       </c>
@@ -7346,7 +7511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>56</v>
       </c>
@@ -7355,7 +7520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>47</v>
       </c>
@@ -7364,16 +7529,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>44</v>
       </c>
       <c r="F27" s="23">
         <f>SUMIF(Activities!B:B,A27,Activities!F:F)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>45</v>
       </c>
@@ -7382,7 +7547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>58</v>
       </c>
@@ -7391,12 +7556,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>40</v>
       </c>
@@ -7427,7 +7592,7 @@
       <c r="J32" s="22"/>
       <c r="K32" s="22"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>46</v>
       </c>
@@ -7456,7 +7621,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>57</v>
       </c>
@@ -7477,7 +7642,7 @@
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>46</v>
       </c>
@@ -7494,7 +7659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>50</v>
       </c>
@@ -7511,7 +7676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>49</v>
       </c>
@@ -7528,7 +7693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>48</v>
       </c>
@@ -7545,7 +7710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>56</v>
       </c>
@@ -7562,7 +7727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>47</v>
       </c>
@@ -7579,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>44</v>
       </c>
@@ -7589,14 +7754,14 @@
       </c>
       <c r="D42" s="23">
         <f>DCOUNT(Activities!A:J,"Estimation Error %",G32:G33)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>45</v>
       </c>
@@ -7613,7 +7778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>58</v>
       </c>
@@ -7630,12 +7795,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>1</v>
       </c>
@@ -7647,7 +7812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>2</v>
       </c>
@@ -7659,7 +7824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>3</v>
       </c>
@@ -7671,7 +7836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>4</v>
       </c>
@@ -7680,10 +7845,10 @@
       </c>
       <c r="F50" s="23">
         <f>SUMIF(Activities!C:C,C50,Activities!F:F)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>5</v>
       </c>
@@ -7695,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>6</v>
       </c>
@@ -7707,7 +7872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>7</v>
       </c>
@@ -7719,7 +7884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>8</v>
       </c>
@@ -7731,7 +7896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>9</v>
       </c>
@@ -7743,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>10</v>
       </c>
@@ -7755,13 +7920,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>68</v>
       </c>
       <c r="F57" s="23">
         <f>SUM(F47:F56)</f>
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -7779,9 +7944,9 @@
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="5:10" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:10" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="E2" s="26" t="s">
         <v>20</v>
       </c>
@@ -7807,77 +7972,77 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="C1" s="31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="C2" s="31"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>

</xml_diff>